<commit_message>
[what] add a Result Report explanation file - with provision of sample input / output files for examination
</commit_message>
<xml_diff>
--- a/complete_system_demo_report.xlsx
+++ b/complete_system_demo_report.xlsx
@@ -1,49 +1,260 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juihungkao/blockchain-based-teais-js/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364B8D80-6016-9145-AB9B-70760695DE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34200" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="PublicBulletinBoard" sheetId="1" r:id="rId1"/>
     <sheet name="CompanyVerifications" sheetId="2" r:id="rId2"/>
     <sheet name="NetworkIntegrity" sheetId="3" r:id="rId3"/>
     <sheet name="VerificationSummary" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+  <si>
+    <t>companyId</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>publicKey</t>
+  </si>
+  <si>
+    <t>declaredSentTotal</t>
+  </si>
+  <si>
+    <t>declaredReceivedTotal</t>
+  </si>
+  <si>
+    <t>homomorphicSentHash</t>
+  </si>
+  <si>
+    <t>homomorphicReceivedHash</t>
+  </si>
+  <si>
+    <t>verificationStatus</t>
+  </si>
+  <si>
+    <t>transactionCount</t>
+  </si>
+  <si>
+    <t>netPosition</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TechCorp Solutions</t>
+  </si>
+  <si>
+    <t>1022117</t>
+  </si>
+  <si>
+    <t>691213956933</t>
+  </si>
+  <si>
+    <t>649539395148</t>
+  </si>
+  <si>
+    <t>GM002</t>
+  </si>
+  <si>
+    <t>Global Manufacturing Inc</t>
+  </si>
+  <si>
+    <t>1040399</t>
+  </si>
+  <si>
+    <t>780042485108</t>
+  </si>
+  <si>
+    <t>704958560562</t>
+  </si>
+  <si>
+    <t>SC003</t>
+  </si>
+  <si>
+    <t>Supply Chain Logistics</t>
+  </si>
+  <si>
+    <t>1065023</t>
+  </si>
+  <si>
+    <t>464937796916</t>
+  </si>
+  <si>
+    <t>600591569499</t>
+  </si>
+  <si>
+    <t>DS004</t>
+  </si>
+  <si>
+    <t>Digital Services Ltd</t>
+  </si>
+  <si>
+    <t>1089911</t>
+  </si>
+  <si>
+    <t>1117443246492</t>
+  </si>
+  <si>
+    <t>152149300430</t>
+  </si>
+  <si>
+    <t>AM005</t>
+  </si>
+  <si>
+    <t>Advanced Materials Co</t>
+  </si>
+  <si>
+    <t>1115111</t>
+  </si>
+  <si>
+    <t>322501967413</t>
+  </si>
+  <si>
+    <t>206071538348</t>
+  </si>
+  <si>
+    <t>RD006</t>
+  </si>
+  <si>
+    <t>Retail Distribution Network</t>
+  </si>
+  <si>
+    <t>1136347</t>
+  </si>
+  <si>
+    <t>595544132993</t>
+  </si>
+  <si>
+    <t>1088075426234</t>
+  </si>
+  <si>
+    <t>FS007</t>
+  </si>
+  <si>
+    <t>Financial Services Group</t>
+  </si>
+  <si>
+    <t>1185917</t>
+  </si>
+  <si>
+    <t>1067772963807</t>
+  </si>
+  <si>
+    <t>419376064103</t>
+  </si>
+  <si>
+    <t>TS008</t>
+  </si>
+  <si>
+    <t>Transportation Systems</t>
+  </si>
+  <si>
+    <t>1199021</t>
+  </si>
+  <si>
+    <t>211287381018</t>
+  </si>
+  <si>
+    <t>424509151031</t>
+  </si>
+  <si>
+    <t>transactionCounts</t>
+  </si>
+  <si>
+    <t>actualSums</t>
+  </si>
+  <si>
+    <t>homomorphicSums</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>verificationDetails</t>
+  </si>
+  <si>
+    <t>totalNetworkVolume</t>
+  </si>
+  <si>
+    <t>totalSent</t>
+  </si>
+  <si>
+    <t>totalReceived</t>
+  </si>
+  <si>
+    <t>networkBalance</t>
+  </si>
+  <si>
+    <t>networkBalanced</t>
+  </si>
+  <si>
+    <t>transactionConsistency</t>
+  </si>
+  <si>
+    <t>uniqueTransactionCount</t>
+  </si>
+  <si>
+    <t>duplicateTransactions</t>
+  </si>
+  <si>
+    <t>allCompaniesVerified</t>
+  </si>
+  <si>
+    <t>totalCompanies</t>
+  </si>
+  <si>
+    <t>totalTransactions</t>
+  </si>
+  <si>
+    <t>companiesVerified</t>
+  </si>
+  <si>
+    <t>systemIntegrity</t>
+  </si>
+  <si>
+    <t>verificationTimestamp</t>
+  </si>
+  <si>
+    <t>VERIFIED</t>
+  </si>
+  <si>
+    <t>2025-10-06T05:25:04.471Z</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -68,13 +279,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -399,65 +618,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>companyId</v>
-      </c>
-      <c r="B1" t="str">
-        <v>companyName</v>
-      </c>
-      <c r="C1" t="str">
-        <v>publicKey</v>
-      </c>
-      <c r="D1" t="str">
-        <v>declaredSentTotal</v>
-      </c>
-      <c r="E1" t="str">
-        <v>declaredReceivedTotal</v>
-      </c>
-      <c r="F1" t="str">
-        <v>homomorphicSentHash</v>
-      </c>
-      <c r="G1" t="str">
-        <v>homomorphicReceivedHash</v>
-      </c>
-      <c r="H1" t="str">
-        <v>verificationStatus</v>
-      </c>
-      <c r="I1" t="str">
-        <v>transactionCount</v>
-      </c>
-      <c r="J1" t="str">
-        <v>netPosition</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>TC001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>TechCorp Solutions</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1022117</v>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
         <v>22800.9</v>
       </c>
       <c r="E2">
-        <v>9500.45</v>
-      </c>
-      <c r="F2" t="str">
-        <v>691213956933</v>
-      </c>
-      <c r="G2" t="str">
-        <v>649539395148</v>
+        <v>9500.4500000000007</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -469,15 +691,15 @@
         <v>-13300.45</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>GM002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Global Manufacturing Inc</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1040399</v>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
       </c>
       <c r="D3">
         <v>25001.25</v>
@@ -485,11 +707,11 @@
       <c r="E3">
         <v>28400.6</v>
       </c>
-      <c r="F3" t="str">
-        <v>780042485108</v>
-      </c>
-      <c r="G3" t="str">
-        <v>704958560562</v>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -501,15 +723,15 @@
         <v>3399.3499999999985</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>SC003</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Supply Chain Logistics</v>
-      </c>
-      <c r="C4" t="str">
-        <v>1065023</v>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
       </c>
       <c r="D4">
         <v>12750.25</v>
@@ -517,11 +739,11 @@
       <c r="E4">
         <v>18400.75</v>
       </c>
-      <c r="F4" t="str">
-        <v>464937796916</v>
-      </c>
-      <c r="G4" t="str">
-        <v>600591569499</v>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -533,15 +755,15 @@
         <v>5650.5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>DS004</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Digital Services Ltd</v>
-      </c>
-      <c r="C5" t="str">
-        <v>1089911</v>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
       </c>
       <c r="D5">
         <v>31901</v>
@@ -549,11 +771,11 @@
       <c r="E5">
         <v>29251</v>
       </c>
-      <c r="F5" t="str">
-        <v>1117443246492</v>
-      </c>
-      <c r="G5" t="str">
-        <v>152149300430</v>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -565,27 +787,27 @@
         <v>-2650</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>AM005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Advanced Materials Co</v>
-      </c>
-      <c r="C6" t="str">
-        <v>1115111</v>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>18400.6</v>
+        <v>18400.599999999999</v>
       </c>
       <c r="E6">
         <v>29801.65</v>
       </c>
-      <c r="F6" t="str">
-        <v>322501967413</v>
-      </c>
-      <c r="G6" t="str">
-        <v>206071538348</v>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
@@ -597,15 +819,15 @@
         <v>11401.050000000003</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>RD006</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Retail Distribution Network</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1136347</v>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
       </c>
       <c r="D7">
         <v>18900.3</v>
@@ -613,11 +835,11 @@
       <c r="E7">
         <v>5000</v>
       </c>
-      <c r="F7" t="str">
-        <v>595544132993</v>
-      </c>
-      <c r="G7" t="str">
-        <v>1088075426234</v>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -629,15 +851,15 @@
         <v>-13900.3</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>FS007</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Financial Services Group</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1185917</v>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
       </c>
       <c r="D8">
         <v>11200.8</v>
@@ -645,11 +867,11 @@
       <c r="E8">
         <v>18900.3</v>
       </c>
-      <c r="F8" t="str">
-        <v>1067772963807</v>
-      </c>
-      <c r="G8" t="str">
-        <v>419376064103</v>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
@@ -661,27 +883,27 @@
         <v>7699.5</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>TS008</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Transportation Systems</v>
-      </c>
-      <c r="C9" t="str">
-        <v>1199021</v>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
       </c>
       <c r="D9">
-        <v>9500.45</v>
+        <v>9500.4500000000007</v>
       </c>
       <c r="E9">
         <v>11200.8</v>
       </c>
-      <c r="F9" t="str">
-        <v>211287381018</v>
-      </c>
-      <c r="G9" t="str">
-        <v>424509151031</v>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -694,174 +916,182 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J9"/>
+    <ignoredError sqref="A1:J9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>companyId</v>
-      </c>
-      <c r="B1" t="str">
-        <v>companyName</v>
-      </c>
-      <c r="C1" t="str">
-        <v>transactionCounts</v>
-      </c>
-      <c r="D1" t="str">
-        <v>actualSums</v>
-      </c>
-      <c r="E1" t="str">
-        <v>homomorphicSums</v>
-      </c>
-      <c r="F1" t="str">
-        <v>verified</v>
-      </c>
-      <c r="G1" t="str">
-        <v>verificationDetails</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>TC001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>TechCorp Solutions</v>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>GM002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Global Manufacturing Inc</v>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>SC003</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Supply Chain Logistics</v>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>DS004</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Digital Services Ltd</v>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>AM005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Advanced Materials Co</v>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>RD006</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Retail Distribution Network</v>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>FS007</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Financial Services Group</v>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>TS008</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Transportation Systems</v>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
+    <ignoredError sqref="A1:G9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>totalNetworkVolume</v>
-      </c>
-      <c r="B1" t="str">
-        <v>totalSent</v>
-      </c>
-      <c r="C1" t="str">
-        <v>totalReceived</v>
-      </c>
-      <c r="D1" t="str">
-        <v>networkBalance</v>
-      </c>
-      <c r="E1" t="str">
-        <v>networkBalanced</v>
-      </c>
-      <c r="F1" t="str">
-        <v>transactionConsistency</v>
-      </c>
-      <c r="G1" t="str">
-        <v>uniqueTransactionCount</v>
-      </c>
-      <c r="H1" t="str">
-        <v>duplicateTransactions</v>
-      </c>
-      <c r="I1" t="str">
-        <v>allCompaniesVerified</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>150455.55000000002</v>
       </c>
@@ -869,10 +1099,10 @@
         <v>150455.55000000002</v>
       </c>
       <c r="C2">
-        <v>150455.55</v>
+        <v>150455.54999999999</v>
       </c>
       <c r="D2">
-        <v>-2.9103830456733704e-11</v>
+        <v>-2.9103830456733704E-11</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -888,43 +1118,46 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError sqref="A1:I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>totalCompanies</v>
-      </c>
-      <c r="B1" t="str">
-        <v>totalTransactions</v>
-      </c>
-      <c r="C1" t="str">
-        <v>companiesVerified</v>
-      </c>
-      <c r="D1" t="str">
-        <v>totalNetworkVolume</v>
-      </c>
-      <c r="E1" t="str">
-        <v>networkBalanced</v>
-      </c>
-      <c r="F1" t="str">
-        <v>systemIntegrity</v>
-      </c>
-      <c r="G1" t="str">
-        <v>verificationTimestamp</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>8</v>
       </c>
@@ -940,16 +1173,18 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="str">
-        <v>VERIFIED</v>
-      </c>
-      <c r="G2" t="str">
-        <v>2025-10-06T05:25:04.471Z</v>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError sqref="A1:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>